<commit_message>
Fix missing image size
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Hand_Siegfried_cours_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9909E8-647A-4488-B81F-FE379F091157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE152BCE-2218-45F3-9823-E10DDDD5EE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="174">
   <si>
     <t>Catégorie</t>
   </si>
@@ -538,6 +538,21 @@
   </si>
   <si>
     <t xml:space="preserve">Redimensionner les images trop volumineuse. Compresser toutes les images. Privilegier le format WebP </t>
+  </si>
+  <si>
+    <t>Les éléments d'image n'ont pas de largeur et de hauteur explicites</t>
+  </si>
+  <si>
+    <t>Cette approche garantit que le navigateur peut allouer la bonne quantité d'espace dans le document pendant le chargement de l'image.</t>
+  </si>
+  <si>
+    <t>Incluez toujours les attributs de taille de largeur et de hauteur sur vos images et éléments vidéo.</t>
+  </si>
+  <si>
+    <t>Ajouter les largeurs et hauteurs aux images</t>
+  </si>
+  <si>
+    <t>https://web.dev/optimize-cls/?utm_source=lighthouse&amp;utm_medium=devtools#images-without-dimensions</t>
   </si>
 </sst>
 </file>
@@ -853,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z42"/>
+  <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1417,21 +1432,24 @@
         <v>150</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>112</v>
+        <v>49</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>54</v>
+        <v>170</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>153</v>
+        <v>172</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1439,30 +1457,30 @@
         <v>112</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>55</v>
+        <v>151</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>56</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>154</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1470,7 +1488,7 @@
         <v>58</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>63</v>
@@ -1484,13 +1502,13 @@
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>155</v>
+        <v>63</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>60</v>
@@ -1499,35 +1517,32 @@
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>112</v>
+        <v>27</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -1535,69 +1550,89 @@
         <v>112</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F40" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="90" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B40" s="3" t="s">
+    <row r="41" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E41" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="F41" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B41" s="3" t="s">
+    <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F42" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="75" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B42" s="3" t="s">
+    <row r="43" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F43" s="5" t="s">
         <v>167</v>
       </c>
     </row>
@@ -1607,14 +1642,15 @@
     <hyperlink ref="F29" r:id="rId2" location="sc1.1.1" xr:uid="{291C747B-F8AA-44D3-AC14-9CE1E3947A1C}"/>
     <hyperlink ref="F2" r:id="rId3" location="sc3.1.1" xr:uid="{555DF8A2-840E-4E4E-BD55-6059FE7B2467}"/>
     <hyperlink ref="F15" r:id="rId4" location="sc1.4.3" xr:uid="{83B6A146-67F2-41CC-A91A-38FFAAF0205C}"/>
-    <hyperlink ref="F38" r:id="rId5" location="sc2.4.4" xr:uid="{622B0E05-3E22-4C9E-A247-E4477A58E199}"/>
-    <hyperlink ref="F39" r:id="rId6" location="sc1.3.1" xr:uid="{684A6670-BB96-43D5-AF5A-2F4E896E80F4}"/>
-    <hyperlink ref="F40" r:id="rId7" location="sc1.1.1" xr:uid="{7281D2C5-7EFA-4D7F-9428-B1FF702BD1D6}"/>
-    <hyperlink ref="F41" r:id="rId8" location="sc2.4.4" xr:uid="{C8BBB30F-20F0-4AA0-83C0-2CCDF354A631}"/>
+    <hyperlink ref="F39" r:id="rId5" location="sc2.4.4" xr:uid="{622B0E05-3E22-4C9E-A247-E4477A58E199}"/>
+    <hyperlink ref="F40" r:id="rId6" location="sc1.3.1" xr:uid="{684A6670-BB96-43D5-AF5A-2F4E896E80F4}"/>
+    <hyperlink ref="F41" r:id="rId7" location="sc1.1.1" xr:uid="{7281D2C5-7EFA-4D7F-9428-B1FF702BD1D6}"/>
+    <hyperlink ref="F42" r:id="rId8" location="sc2.4.4" xr:uid="{C8BBB30F-20F0-4AA0-83C0-2CCDF354A631}"/>
     <hyperlink ref="F14" r:id="rId9" xr:uid="{FC8B2372-F881-4853-BC8B-433E85A2790A}"/>
-    <hyperlink ref="F42" r:id="rId10" xr:uid="{0EC693F2-99ED-4BC3-B225-FBDCDA302BDF}"/>
+    <hyperlink ref="F43" r:id="rId10" xr:uid="{0EC693F2-99ED-4BC3-B225-FBDCDA302BDF}"/>
+    <hyperlink ref="F32" r:id="rId11" location="images-without-dimensions" xr:uid="{931F68BF-F3AE-4266-8EBC-3EA2F62C0FC1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId11"/>
+  <pageSetup orientation="landscape" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Use CDN for performances
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Hand_Siegfried_cours_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE152BCE-2218-45F3-9823-E10DDDD5EE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB34A07B-D6EC-44CC-8504-FDE01CA006C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="178">
   <si>
     <t>Catégorie</t>
   </si>
@@ -553,6 +553,18 @@
   </si>
   <si>
     <t>https://web.dev/optimize-cls/?utm_source=lighthouse&amp;utm_medium=devtools#images-without-dimensions</t>
+  </si>
+  <si>
+    <t>Le chargement de Boostrap.js et JQuery.js ralentisse le chargement de la page.</t>
+  </si>
+  <si>
+    <t>De nombreux utilisateurs ont déjà téléchargé Bootstrap à partir de MaxCDN lorsqu'ils visitent un autre site. En conséquence, il sera chargé à partir du cache lorsqu'ils visiteront votre site, ce qui accélérera le temps de chargement. De plus, la plupart des CDN s'assureront qu'une fois qu'un utilisateur lui demande un fichier, il sera servi à partir du serveur le plus proche, ce qui entraîne également un temps de chargement plus rapide.</t>
+  </si>
+  <si>
+    <t>Utiliser un CDN pour Boostrap et Jquery.</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/bootstrap/bootstrap_get_started.asp</t>
   </si>
 </sst>
 </file>
@@ -868,7 +880,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z43"/>
+  <dimension ref="A1:Z44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
@@ -1432,41 +1444,41 @@
         <v>150</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F33" s="5" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1474,30 +1486,30 @@
         <v>112</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>55</v>
+        <v>151</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>56</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>154</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1505,7 +1517,7 @@
         <v>58</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>63</v>
@@ -1519,13 +1531,13 @@
     </row>
     <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>155</v>
+        <v>63</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>60</v>
@@ -1534,35 +1546,32 @@
         <v>154</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>112</v>
+        <v>27</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -1570,69 +1579,89 @@
         <v>112</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E41" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="F41" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="90" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B41" s="3" t="s">
+    <row r="42" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F42" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B42" s="3" t="s">
+    <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F43" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="75" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B43" s="3" t="s">
+    <row r="44" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="F44" s="5" t="s">
         <v>167</v>
       </c>
     </row>
@@ -1642,15 +1671,16 @@
     <hyperlink ref="F29" r:id="rId2" location="sc1.1.1" xr:uid="{291C747B-F8AA-44D3-AC14-9CE1E3947A1C}"/>
     <hyperlink ref="F2" r:id="rId3" location="sc3.1.1" xr:uid="{555DF8A2-840E-4E4E-BD55-6059FE7B2467}"/>
     <hyperlink ref="F15" r:id="rId4" location="sc1.4.3" xr:uid="{83B6A146-67F2-41CC-A91A-38FFAAF0205C}"/>
-    <hyperlink ref="F39" r:id="rId5" location="sc2.4.4" xr:uid="{622B0E05-3E22-4C9E-A247-E4477A58E199}"/>
-    <hyperlink ref="F40" r:id="rId6" location="sc1.3.1" xr:uid="{684A6670-BB96-43D5-AF5A-2F4E896E80F4}"/>
-    <hyperlink ref="F41" r:id="rId7" location="sc1.1.1" xr:uid="{7281D2C5-7EFA-4D7F-9428-B1FF702BD1D6}"/>
-    <hyperlink ref="F42" r:id="rId8" location="sc2.4.4" xr:uid="{C8BBB30F-20F0-4AA0-83C0-2CCDF354A631}"/>
+    <hyperlink ref="F40" r:id="rId5" location="sc2.4.4" xr:uid="{622B0E05-3E22-4C9E-A247-E4477A58E199}"/>
+    <hyperlink ref="F41" r:id="rId6" location="sc1.3.1" xr:uid="{684A6670-BB96-43D5-AF5A-2F4E896E80F4}"/>
+    <hyperlink ref="F42" r:id="rId7" location="sc1.1.1" xr:uid="{7281D2C5-7EFA-4D7F-9428-B1FF702BD1D6}"/>
+    <hyperlink ref="F43" r:id="rId8" location="sc2.4.4" xr:uid="{C8BBB30F-20F0-4AA0-83C0-2CCDF354A631}"/>
     <hyperlink ref="F14" r:id="rId9" xr:uid="{FC8B2372-F881-4853-BC8B-433E85A2790A}"/>
-    <hyperlink ref="F43" r:id="rId10" xr:uid="{0EC693F2-99ED-4BC3-B225-FBDCDA302BDF}"/>
-    <hyperlink ref="F32" r:id="rId11" location="images-without-dimensions" xr:uid="{931F68BF-F3AE-4266-8EBC-3EA2F62C0FC1}"/>
+    <hyperlink ref="F44" r:id="rId10" xr:uid="{0EC693F2-99ED-4BC3-B225-FBDCDA302BDF}"/>
+    <hyperlink ref="F33" r:id="rId11" location="images-without-dimensions" xr:uid="{931F68BF-F3AE-4266-8EBC-3EA2F62C0FC1}"/>
+    <hyperlink ref="F32" r:id="rId12" xr:uid="{D229EC8C-CF0D-40EA-BBEC-EEE2E1293098}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId12"/>
+  <pageSetup orientation="landscape" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Page links tag fix
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Hand_Siegfried_cours_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB34A07B-D6EC-44CC-8504-FDE01CA006C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046E5160-079A-4880-9871-C4F124A399E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="181">
   <si>
     <t>Catégorie</t>
   </si>
@@ -565,6 +565,15 @@
   </si>
   <si>
     <t>https://www.w3schools.com/bootstrap/bootstrap_get_started.asp</t>
+  </si>
+  <si>
+    <t>Sue la page2.html les liens css ne sont pas valides</t>
+  </si>
+  <si>
+    <t>les liens pointent vers .min.css</t>
+  </si>
+  <si>
+    <t>Corriger les liens</t>
   </si>
 </sst>
 </file>
@@ -880,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z44"/>
+  <dimension ref="A1:Z45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1006,320 +1015,317 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="90" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="90" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>15</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>19</v>
+        <v>107</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>109</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+    <row r="15" spans="1:26" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+    <row r="16" spans="1:26" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F16" s="5" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="30" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F17" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>119</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>112</v>
+        <v>6</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>125</v>
+        <v>34</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>36</v>
+        <v>123</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>127</v>
+        <v>36</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1327,16 +1333,16 @@
         <v>112</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1344,16 +1350,16 @@
         <v>112</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>39</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1361,16 +1367,16 @@
         <v>112</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>143</v>
+        <v>38</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>144</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1378,16 +1384,16 @@
         <v>112</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>40</v>
+        <v>142</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>145</v>
+        <v>53</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>41</v>
+        <v>143</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>42</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1395,36 +1401,36 @@
         <v>112</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>44</v>
+        <v>145</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>49</v>
+        <v>112</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>146</v>
+        <v>44</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>147</v>
+        <v>46</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1432,70 +1438,70 @@
         <v>49</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>174</v>
+        <v>52</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>175</v>
+        <v>148</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F34" s="5" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1503,30 +1509,30 @@
         <v>112</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>55</v>
+        <v>151</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>56</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>154</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1534,7 +1540,7 @@
         <v>58</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>63</v>
@@ -1548,13 +1554,13 @@
     </row>
     <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>155</v>
+        <v>63</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>60</v>
@@ -1563,35 +1569,32 @@
         <v>154</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>112</v>
+        <v>27</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>156</v>
+        <v>62</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>69</v>
+        <v>156</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>72</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -1599,86 +1602,106 @@
         <v>112</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="90" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D45" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E45" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F45" s="5" t="s">
         <v>167</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F16" r:id="rId1" xr:uid="{E96C1179-36DF-4C39-B71F-14345EDAD9C5}"/>
-    <hyperlink ref="F29" r:id="rId2" location="sc1.1.1" xr:uid="{291C747B-F8AA-44D3-AC14-9CE1E3947A1C}"/>
+    <hyperlink ref="F17" r:id="rId1" xr:uid="{E96C1179-36DF-4C39-B71F-14345EDAD9C5}"/>
+    <hyperlink ref="F30" r:id="rId2" location="sc1.1.1" xr:uid="{291C747B-F8AA-44D3-AC14-9CE1E3947A1C}"/>
     <hyperlink ref="F2" r:id="rId3" location="sc3.1.1" xr:uid="{555DF8A2-840E-4E4E-BD55-6059FE7B2467}"/>
-    <hyperlink ref="F15" r:id="rId4" location="sc1.4.3" xr:uid="{83B6A146-67F2-41CC-A91A-38FFAAF0205C}"/>
-    <hyperlink ref="F40" r:id="rId5" location="sc2.4.4" xr:uid="{622B0E05-3E22-4C9E-A247-E4477A58E199}"/>
-    <hyperlink ref="F41" r:id="rId6" location="sc1.3.1" xr:uid="{684A6670-BB96-43D5-AF5A-2F4E896E80F4}"/>
-    <hyperlink ref="F42" r:id="rId7" location="sc1.1.1" xr:uid="{7281D2C5-7EFA-4D7F-9428-B1FF702BD1D6}"/>
-    <hyperlink ref="F43" r:id="rId8" location="sc2.4.4" xr:uid="{C8BBB30F-20F0-4AA0-83C0-2CCDF354A631}"/>
-    <hyperlink ref="F14" r:id="rId9" xr:uid="{FC8B2372-F881-4853-BC8B-433E85A2790A}"/>
-    <hyperlink ref="F44" r:id="rId10" xr:uid="{0EC693F2-99ED-4BC3-B225-FBDCDA302BDF}"/>
-    <hyperlink ref="F33" r:id="rId11" location="images-without-dimensions" xr:uid="{931F68BF-F3AE-4266-8EBC-3EA2F62C0FC1}"/>
-    <hyperlink ref="F32" r:id="rId12" xr:uid="{D229EC8C-CF0D-40EA-BBEC-EEE2E1293098}"/>
+    <hyperlink ref="F16" r:id="rId4" location="sc1.4.3" xr:uid="{83B6A146-67F2-41CC-A91A-38FFAAF0205C}"/>
+    <hyperlink ref="F41" r:id="rId5" location="sc2.4.4" xr:uid="{622B0E05-3E22-4C9E-A247-E4477A58E199}"/>
+    <hyperlink ref="F42" r:id="rId6" location="sc1.3.1" xr:uid="{684A6670-BB96-43D5-AF5A-2F4E896E80F4}"/>
+    <hyperlink ref="F43" r:id="rId7" location="sc1.1.1" xr:uid="{7281D2C5-7EFA-4D7F-9428-B1FF702BD1D6}"/>
+    <hyperlink ref="F44" r:id="rId8" location="sc2.4.4" xr:uid="{C8BBB30F-20F0-4AA0-83C0-2CCDF354A631}"/>
+    <hyperlink ref="F15" r:id="rId9" xr:uid="{FC8B2372-F881-4853-BC8B-433E85A2790A}"/>
+    <hyperlink ref="F45" r:id="rId10" xr:uid="{0EC693F2-99ED-4BC3-B225-FBDCDA302BDF}"/>
+    <hyperlink ref="F34" r:id="rId11" location="images-without-dimensions" xr:uid="{931F68BF-F3AE-4266-8EBC-3EA2F62C0FC1}"/>
+    <hyperlink ref="F33" r:id="rId12" xr:uid="{D229EC8C-CF0D-40EA-BBEC-EEE2E1293098}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId13"/>

</xml_diff>

<commit_message>
Fix bootstrap validation fix
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Hand_Siegfried_cours_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046E5160-079A-4880-9871-C4F124A399E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF54138-D2BD-4DCF-909D-882755101728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="182">
   <si>
     <t>Catégorie</t>
   </si>
@@ -574,6 +574,9 @@
   </si>
   <si>
     <t>Corriger les liens</t>
+  </si>
+  <si>
+    <t>La propriétés de media max-device-width est déconseillée. Pour plus d'information, regardez la section "Deprecated Media Features" dans la version actuelle de la spécification Media Queries.</t>
   </si>
 </sst>
 </file>
@@ -891,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1535,7 +1538,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>58</v>
       </c>
@@ -1543,7 +1546,7 @@
         <v>59</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>63</v>
+        <v>181</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>60</v>

</xml_diff>